<commit_message>
Cubiertas horas de octubre
</commit_message>
<xml_diff>
--- a/TimeSheets/TS-DII-RRD-13-10.xlsx
+++ b/TimeSheets/TS-DII-RRD-13-10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="151" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="100" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -126,45 +126,45 @@
   </numFmts>
   <fonts count="7">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="9"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -336,96 +336,161 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="39">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="8" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="9" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="12" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="14" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="15" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="16" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="17" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="17" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="18" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="4" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -447,14 +512,15 @@
   <dimension ref="A1:AF35"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
+      <selection activeCell="AI24" activeCellId="0" pane="topLeft" sqref="AI24"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.2745098039216"/>
-    <col collapsed="false" hidden="false" max="32" min="2" style="0" width="4.32156862745098"/>
-    <col collapsed="false" hidden="false" max="34" min="33" style="0" width="3.74509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="9.23529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.280612244898"/>
+    <col collapsed="false" hidden="false" max="32" min="2" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="34" min="33" style="0" width="3.74489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="9.23469387755102"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -517,7 +583,7 @@
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -732,75 +798,75 @@
         <v>14</v>
       </c>
       <c r="B11" s="13" t="n">
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="C11" s="13" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D11" s="13" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="13" t="n">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13" t="n">
-        <v>8</v>
+        <v>8.25</v>
       </c>
       <c r="I11" s="13" t="n">
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="J11" s="13" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K11" s="13" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L11" s="13" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13" t="n">
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="P11" s="13" t="n">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="Q11" s="13" t="n">
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="R11" s="13" t="n">
         <v>8</v>
       </c>
       <c r="S11" s="13" t="n">
-        <v>8</v>
+        <v>4.5</v>
       </c>
       <c r="T11" s="13"/>
       <c r="U11" s="13"/>
       <c r="V11" s="13" t="n">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="W11" s="13" t="n">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="X11" s="13" t="n">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="Y11" s="13" t="n">
         <v>8</v>
       </c>
       <c r="Z11" s="13" t="n">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="AA11" s="13"/>
       <c r="AB11" s="13"/>
       <c r="AC11" s="13" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AD11" s="13" t="n">
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="AE11" s="13" t="n">
         <v>8</v>
@@ -1031,19 +1097,19 @@
       </c>
       <c r="B18" s="18" t="n">
         <f aca="false">SUM(B11:B17)</f>
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="C18" s="18" t="n">
         <f aca="false">SUM(C11:C17)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D18" s="18" t="n">
         <f aca="false">SUM(D11:D17)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E18" s="18" t="n">
         <f aca="false">SUM(E11:E17)</f>
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="F18" s="18" t="n">
         <f aca="false">SUM(F11:F17)</f>
@@ -1055,23 +1121,23 @@
       </c>
       <c r="H18" s="18" t="n">
         <f aca="false">SUM(H11:H17)</f>
-        <v>8</v>
+        <v>8.25</v>
       </c>
       <c r="I18" s="18" t="n">
         <f aca="false">SUM(I11:I17)</f>
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="J18" s="18" t="n">
         <f aca="false">SUM(J11:J17)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K18" s="18" t="n">
         <f aca="false">SUM(K11:K17)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L18" s="18" t="n">
         <f aca="false">SUM(L11:L17)</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M18" s="18" t="n">
         <f aca="false">SUM(M11:M17)</f>
@@ -1083,15 +1149,15 @@
       </c>
       <c r="O18" s="18" t="n">
         <f aca="false">SUM(O11:O17)</f>
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="P18" s="18" t="n">
         <f aca="false">SUM(P11:P17)</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="Q18" s="18" t="n">
         <f aca="false">SUM(Q11:Q17)</f>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="R18" s="18" t="n">
         <f aca="false">SUM(R11:R17)</f>
@@ -1099,7 +1165,7 @@
       </c>
       <c r="S18" s="18" t="n">
         <f aca="false">SUM(S11:S17)</f>
-        <v>8</v>
+        <v>4.5</v>
       </c>
       <c r="T18" s="18" t="n">
         <f aca="false">SUM(T11:T17)</f>
@@ -1111,15 +1177,15 @@
       </c>
       <c r="V18" s="18" t="n">
         <f aca="false">SUM(V11:V17)</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="W18" s="18" t="n">
         <f aca="false">SUM(W11:W17)</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="X18" s="18" t="n">
         <f aca="false">SUM(X11:X17)</f>
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="Y18" s="18" t="n">
         <f aca="false">SUM(Y11:Y17)</f>
@@ -1127,7 +1193,7 @@
       </c>
       <c r="Z18" s="18" t="n">
         <f aca="false">SUM(Z11:Z17)</f>
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="AA18" s="18" t="n">
         <f aca="false">SUM(AA11:AA17)</f>
@@ -1139,11 +1205,11 @@
       </c>
       <c r="AC18" s="18" t="n">
         <f aca="false">SUM(AC11:AC17)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AD18" s="18" t="n">
         <f aca="false">SUM(AD11:AD17)</f>
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="AE18" s="18" t="n">
         <f aca="false">SUM(AE11:AE17)</f>
@@ -1203,7 +1269,7 @@
       <c r="AD23" s="26"/>
       <c r="AE23" s="27" t="n">
         <f aca="false">SUM(B11:AF11)</f>
-        <v>184</v>
+        <v>184.25</v>
       </c>
       <c r="AF23" s="27"/>
     </row>
@@ -1364,7 +1430,7 @@
       <c r="AD30" s="32"/>
       <c r="AE30" s="33" t="n">
         <f aca="false">SUM(AE23:AF29)</f>
-        <v>184</v>
+        <v>184.25</v>
       </c>
       <c r="AF30" s="33"/>
     </row>
@@ -1467,8 +1533,9 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.23529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.23469387755102"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1492,8 +1559,9 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.23529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.23469387755102"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Modificando horas del mes
</commit_message>
<xml_diff>
--- a/TimeSheets/TS-DII-RRD-13-10.xlsx
+++ b/TimeSheets/TS-DII-RRD-13-10.xlsx
@@ -337,7 +337,7 @@
   <dimension ref="A1:AF35"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="AG11" activeCellId="0" pane="topLeft" sqref="AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -623,75 +623,75 @@
         <v>14</v>
       </c>
       <c r="B11" s="7" t="n">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="C11" s="7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11" s="7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="7" t="n">
-        <v>2.5</v>
+        <v>8</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7" t="n">
-        <v>8.25</v>
+        <v>8</v>
       </c>
       <c r="I11" s="7" t="n">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="J11" s="7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K11" s="7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L11" s="7" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7" t="n">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="P11" s="7" t="n">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="Q11" s="7" t="n">
-        <v>10.5</v>
+        <v>8</v>
       </c>
       <c r="R11" s="7" t="n">
         <v>8</v>
       </c>
       <c r="S11" s="7" t="n">
-        <v>4.5</v>
+        <v>8</v>
       </c>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
       <c r="V11" s="7" t="n">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="W11" s="7" t="n">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="X11" s="7" t="n">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="Y11" s="7" t="n">
         <v>8</v>
       </c>
       <c r="Z11" s="7" t="n">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="AA11" s="7"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AD11" s="7" t="n">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="AE11" s="7" t="n">
         <v>8</v>
@@ -922,19 +922,19 @@
       </c>
       <c r="B18" s="7" t="n">
         <f aca="false">SUM(B11:B17)</f>
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="C18" s="7" t="n">
         <f aca="false">SUM(C11:C17)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D18" s="7" t="n">
         <f aca="false">SUM(D11:D17)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="7" t="n">
         <f aca="false">SUM(E11:E17)</f>
-        <v>2.5</v>
+        <v>8</v>
       </c>
       <c r="F18" s="7" t="n">
         <f aca="false">SUM(F11:F17)</f>
@@ -946,23 +946,23 @@
       </c>
       <c r="H18" s="7" t="n">
         <f aca="false">SUM(H11:H17)</f>
-        <v>8.25</v>
+        <v>8</v>
       </c>
       <c r="I18" s="7" t="n">
         <f aca="false">SUM(I11:I17)</f>
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="J18" s="7" t="n">
         <f aca="false">SUM(J11:J17)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K18" s="7" t="n">
         <f aca="false">SUM(K11:K17)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L18" s="7" t="n">
         <f aca="false">SUM(L11:L17)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M18" s="7" t="n">
         <f aca="false">SUM(M11:M17)</f>
@@ -974,15 +974,15 @@
       </c>
       <c r="O18" s="7" t="n">
         <f aca="false">SUM(O11:O17)</f>
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="P18" s="7" t="n">
         <f aca="false">SUM(P11:P17)</f>
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="Q18" s="7" t="n">
         <f aca="false">SUM(Q11:Q17)</f>
-        <v>10.5</v>
+        <v>8</v>
       </c>
       <c r="R18" s="7" t="n">
         <f aca="false">SUM(R11:R17)</f>
@@ -990,7 +990,7 @@
       </c>
       <c r="S18" s="7" t="n">
         <f aca="false">SUM(S11:S17)</f>
-        <v>4.5</v>
+        <v>8</v>
       </c>
       <c r="T18" s="7" t="n">
         <f aca="false">SUM(T11:T17)</f>
@@ -1002,15 +1002,15 @@
       </c>
       <c r="V18" s="7" t="n">
         <f aca="false">SUM(V11:V17)</f>
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="W18" s="7" t="n">
         <f aca="false">SUM(W11:W17)</f>
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="X18" s="7" t="n">
         <f aca="false">SUM(X11:X17)</f>
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="Y18" s="7" t="n">
         <f aca="false">SUM(Y11:Y17)</f>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="Z18" s="7" t="n">
         <f aca="false">SUM(Z11:Z17)</f>
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="AA18" s="7" t="n">
         <f aca="false">SUM(AA11:AA17)</f>
@@ -1030,11 +1030,11 @@
       </c>
       <c r="AC18" s="7" t="n">
         <f aca="false">SUM(AC11:AC17)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AD18" s="7" t="n">
         <f aca="false">SUM(AD11:AD17)</f>
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="AE18" s="7" t="n">
         <f aca="false">SUM(AE11:AE17)</f>
@@ -1094,7 +1094,7 @@
       <c r="AD23" s="14"/>
       <c r="AE23" s="15" t="n">
         <f aca="false">SUM(B11:AF11)</f>
-        <v>184.25</v>
+        <v>184</v>
       </c>
       <c r="AF23" s="15"/>
     </row>
@@ -1255,7 +1255,7 @@
       <c r="AD30" s="18"/>
       <c r="AE30" s="19" t="n">
         <f aca="false">SUM(AE23:AF29)</f>
-        <v>184.25</v>
+        <v>184</v>
       </c>
       <c r="AF30" s="19"/>
     </row>

</xml_diff>